<commit_message>
Auto-committed on 2021/11/30 週二
Former-commit-id: 1a85d9c2f566544b7cbc4f1f280bf84280d6b513
</commit_message>
<xml_diff>
--- a/Program/Other/LM076_底稿_B042金融機構承作「購地貸款」統計表.xlsx
+++ b/Program/Other/LM076_底稿_B042金融機構承作「購地貸款」統計表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN_REPO_SKL\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA09BF90-3E86-43B8-AC6F-F79F52A64AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84AE264-764B-410C-BB4F-BC09EEF8D0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1799,84 +1799,84 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="37" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="177" fontId="36" fillId="30" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="37" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="177" fontId="36" fillId="30" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -2274,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF65552-3C83-45D0-BB5D-33C0B60BEEF0}">
-  <dimension ref="A1:BQ25"/>
+  <dimension ref="A1:BP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -2290,7 +2290,7 @@
     <col min="6" max="6" width="20.33203125" style="12" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" style="12" customWidth="1"/>
     <col min="8" max="9" width="19.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="45" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="37" customWidth="1"/>
     <col min="11" max="16" width="13.77734375" style="12" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="7.33203125" style="12" hidden="1" customWidth="1"/>
     <col min="18" max="20" width="13.77734375" style="12" hidden="1" customWidth="1"/>
@@ -2304,16 +2304,16 @@
         <f>IF(COUNTBLANK(I7:I14)=8,"","本表有誤")</f>
         <v/>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="45"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="37"/>
       <c r="BG1" s="7" t="e">
         <f>SUBSTITUTE(SUBSTITUTE(#REF!," ",""),"　","")</f>
         <v>#REF!</v>
@@ -2351,178 +2351,178 @@
       </c>
     </row>
     <row r="2" spans="1:68" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="C2" s="56" t="s">
+      <c r="A2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
-      <c r="AL2" s="55"/>
-      <c r="AM2" s="55"/>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="55"/>
-      <c r="AQ2" s="55"/>
-      <c r="AR2" s="55"/>
-      <c r="AS2" s="55"/>
-      <c r="AT2" s="55"/>
-      <c r="AU2" s="55"/>
-      <c r="AV2" s="55"/>
-      <c r="AW2" s="55"/>
-      <c r="AX2" s="55"/>
-      <c r="AY2" s="55"/>
-      <c r="AZ2" s="55"/>
-      <c r="BA2" s="55"/>
-      <c r="BB2" s="55"/>
-      <c r="BC2" s="55"/>
-      <c r="BD2" s="55"/>
-      <c r="BE2" s="55"/>
-      <c r="BF2" s="55"/>
-      <c r="BG2" s="55"/>
-      <c r="BH2" s="55"/>
-      <c r="BI2" s="55"/>
-      <c r="BJ2" s="55"/>
-      <c r="BK2" s="55"/>
-      <c r="BL2" s="55"/>
-      <c r="BM2" s="55"/>
-      <c r="BN2" s="55"/>
-      <c r="BO2" s="55"/>
-      <c r="BP2" s="55"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+      <c r="BA2" s="38"/>
+      <c r="BB2" s="38"/>
+      <c r="BC2" s="38"/>
+      <c r="BD2" s="38"/>
+      <c r="BE2" s="38"/>
+      <c r="BF2" s="38"/>
+      <c r="BG2" s="38"/>
+      <c r="BH2" s="38"/>
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="38"/>
+      <c r="BK2" s="38"/>
+      <c r="BL2" s="38"/>
+      <c r="BM2" s="38"/>
+      <c r="BN2" s="38"/>
+      <c r="BO2" s="38"/>
+      <c r="BP2" s="38"/>
     </row>
     <row r="3" spans="1:68" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="C3" s="57" t="s">
+      <c r="A3" s="38"/>
+      <c r="C3" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="55"/>
-      <c r="AO3" s="55"/>
-      <c r="AP3" s="55"/>
-      <c r="AQ3" s="55"/>
-      <c r="AR3" s="55"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
-      <c r="AU3" s="55"/>
-      <c r="AV3" s="55"/>
-      <c r="AW3" s="55"/>
-      <c r="AX3" s="55"/>
-      <c r="AY3" s="55"/>
-      <c r="AZ3" s="55"/>
-      <c r="BA3" s="55"/>
-      <c r="BB3" s="55"/>
-      <c r="BC3" s="55"/>
-      <c r="BD3" s="55"/>
-      <c r="BE3" s="55"/>
-      <c r="BF3" s="55"/>
-      <c r="BG3" s="55"/>
-      <c r="BH3" s="55"/>
-      <c r="BI3" s="55"/>
-      <c r="BJ3" s="55"/>
-      <c r="BK3" s="55"/>
-      <c r="BL3" s="55"/>
-      <c r="BM3" s="55"/>
-      <c r="BN3" s="55"/>
-      <c r="BO3" s="55"/>
-      <c r="BP3" s="55"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
+      <c r="AL3" s="38"/>
+      <c r="AM3" s="38"/>
+      <c r="AN3" s="38"/>
+      <c r="AO3" s="38"/>
+      <c r="AP3" s="38"/>
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="38"/>
+      <c r="AS3" s="38"/>
+      <c r="AT3" s="38"/>
+      <c r="AU3" s="38"/>
+      <c r="AV3" s="38"/>
+      <c r="AW3" s="38"/>
+      <c r="AX3" s="38"/>
+      <c r="AY3" s="38"/>
+      <c r="AZ3" s="38"/>
+      <c r="BA3" s="38"/>
+      <c r="BB3" s="38"/>
+      <c r="BC3" s="38"/>
+      <c r="BD3" s="38"/>
+      <c r="BE3" s="38"/>
+      <c r="BF3" s="38"/>
+      <c r="BG3" s="38"/>
+      <c r="BH3" s="38"/>
+      <c r="BI3" s="38"/>
+      <c r="BJ3" s="38"/>
+      <c r="BK3" s="38"/>
+      <c r="BL3" s="38"/>
+      <c r="BM3" s="38"/>
+      <c r="BN3" s="38"/>
+      <c r="BO3" s="38"/>
+      <c r="BP3" s="38"/>
     </row>
     <row r="4" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="53" t="s">
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="53" t="s">
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="53" t="s">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="54"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
     </row>
     <row r="6" spans="1:68" s="13" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="44" t="s">
+      <c r="A6" s="55"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="36" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -2531,7 +2531,7 @@
       <c r="E6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="36" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="20" t="s">
@@ -2540,11 +2540,11 @@
       <c r="H6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="44" t="s">
+      <c r="J6" s="51"/>
+      <c r="K6" s="36" t="s">
         <v>10</v>
       </c>
       <c r="L6" s="14" t="s">
@@ -2553,7 +2553,7 @@
       <c r="M6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="36" t="s">
         <v>10</v>
       </c>
       <c r="O6" s="14" t="s">
@@ -2581,41 +2581,41 @@
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="34"/>
-      <c r="E7" s="58"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="49" t="str">
+      <c r="I7" s="46" t="str">
         <f>$K7&amp;$L7&amp;$M7&amp;$N7&amp;$O7&amp;$P7</f>
         <v/>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="47"/>
       <c r="K7" s="15" t="str">
-        <f>IF(C7="","",IF(OR(C7&lt;0,C7&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C7&lt;&gt;ROUND(C7,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" ref="K7:K14" si="0">IF(C7="","",IF(OR(C7&lt;0,C7&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C7&lt;&gt;ROUND(C7,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
         <v/>
       </c>
       <c r="L7" s="15" t="str">
-        <f>IF(D7="","",IF(D7&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D7&lt;&gt;ROUND(D7,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" ref="L7:L14" si="1">IF(D7="","",IF(D7&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D7&lt;&gt;ROUND(D7,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
         <v/>
       </c>
       <c r="M7" s="15" t="str">
-        <f>IF(E7="","",IF(E7&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E7&lt;&gt;ROUND(E7,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" ref="M7:M14" si="2">IF(E7="","",IF(E7&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E7&lt;&gt;ROUND(E7,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
         <v/>
       </c>
       <c r="N7" s="15" t="str">
-        <f>IF(F7="","",IF(OR(F7&lt;0,F7&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F7&lt;&gt;ROUND(F7,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" ref="N7:N14" si="3">IF(F7="","",IF(OR(F7&lt;0,F7&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F7&lt;&gt;ROUND(F7,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
         <v/>
       </c>
       <c r="O7" s="15" t="str">
-        <f>IF(G7="","",IF(G7&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G7&lt;&gt;ROUND(G7,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" ref="O7:O14" si="4">IF(G7="","",IF(G7&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G7&lt;&gt;ROUND(G7,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
         <v/>
       </c>
       <c r="P7" s="15" t="str">
-        <f>IF(H7="","",IF(H7&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H7&lt;&gt;ROUND(H7,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" ref="P7:P14" si="5">IF(H7="","",IF(H7&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H7&lt;&gt;ROUND(H7,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
         <v/>
       </c>
       <c r="S7" s="16" t="str">
-        <f>IF(L7="",IF(D7&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" ref="S7:S13" si="6">IF(L7="",IF(D7&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
         <v/>
       </c>
     </row>
@@ -2628,41 +2628,41 @@
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
-      <c r="E8" s="58"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
-      <c r="I8" s="49" t="str">
-        <f t="shared" ref="I8:I14" si="0">$K8&amp;$L8&amp;$M8&amp;$N8&amp;$O8&amp;$P8</f>
-        <v/>
-      </c>
-      <c r="J8" s="50"/>
+      <c r="I8" s="46" t="str">
+        <f t="shared" ref="I8:I14" si="7">$K8&amp;$L8&amp;$M8&amp;$N8&amp;$O8&amp;$P8</f>
+        <v/>
+      </c>
+      <c r="J8" s="47"/>
       <c r="K8" s="15" t="str">
-        <f>IF(C8="","",IF(OR(C8&lt;0,C8&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C8&lt;&gt;ROUND(C8,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L8" s="15" t="str">
-        <f>IF(D8="","",IF(D8&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D8&lt;&gt;ROUND(D8,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M8" s="15" t="str">
-        <f>IF(E8="","",IF(E8&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E8&lt;&gt;ROUND(E8,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N8" s="15" t="str">
-        <f>IF(F8="","",IF(OR(F8&lt;0,F8&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F8&lt;&gt;ROUND(F8,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O8" s="15" t="str">
-        <f>IF(G8="","",IF(G8&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G8&lt;&gt;ROUND(G8,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P8" s="15" t="str">
-        <f>IF(H8="","",IF(H8&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H8&lt;&gt;ROUND(H8,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S8" s="16" t="str">
-        <f>IF(L8="",IF(D8&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2675,41 +2675,41 @@
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="34"/>
-      <c r="E9" s="58"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="33"/>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="49" t="str">
+      <c r="I9" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="K9" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J9" s="50"/>
-      <c r="K9" s="15" t="str">
-        <f>IF(C9="","",IF(OR(C9&lt;0,C9&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C9&lt;&gt;ROUND(C9,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L9" s="15" t="str">
-        <f>IF(D9="","",IF(D9&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D9&lt;&gt;ROUND(D9,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M9" s="15" t="str">
-        <f>IF(E9="","",IF(E9&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E9&lt;&gt;ROUND(E9,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N9" s="15" t="str">
-        <f>IF(F9="","",IF(OR(F9&lt;0,F9&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F9&lt;&gt;ROUND(F9,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O9" s="15" t="str">
-        <f>IF(G9="","",IF(G9&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G9&lt;&gt;ROUND(G9,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P9" s="15" t="str">
-        <f>IF(H9="","",IF(H9&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H9&lt;&gt;ROUND(H9,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S9" s="16" t="str">
-        <f>IF(L9="",IF(D9&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2722,41 +2722,41 @@
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="34"/>
-      <c r="E10" s="58"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="33"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="49" t="str">
+      <c r="I10" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="15" t="str">
-        <f>IF(C10="","",IF(OR(C10&lt;0,C10&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C10&lt;&gt;ROUND(C10,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L10" s="15" t="str">
-        <f>IF(D10="","",IF(D10&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D10&lt;&gt;ROUND(D10,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M10" s="15" t="str">
-        <f>IF(E10="","",IF(E10&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E10&lt;&gt;ROUND(E10,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N10" s="15" t="str">
-        <f>IF(F10="","",IF(OR(F10&lt;0,F10&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F10&lt;&gt;ROUND(F10,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O10" s="15" t="str">
-        <f>IF(G10="","",IF(G10&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G10&lt;&gt;ROUND(G10,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P10" s="15" t="str">
-        <f>IF(H10="","",IF(H10&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H10&lt;&gt;ROUND(H10,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S10" s="16" t="str">
-        <f>IF(L10="",IF(D10&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2769,41 +2769,41 @@
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34"/>
-      <c r="E11" s="58"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="33"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="49" t="str">
+      <c r="I11" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J11" s="47"/>
+      <c r="K11" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="15" t="str">
-        <f>IF(C11="","",IF(OR(C11&lt;0,C11&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C11&lt;&gt;ROUND(C11,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L11" s="15" t="str">
-        <f>IF(D11="","",IF(D11&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D11&lt;&gt;ROUND(D11,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M11" s="15" t="str">
-        <f>IF(E11="","",IF(E11&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E11&lt;&gt;ROUND(E11,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N11" s="15" t="str">
-        <f>IF(F11="","",IF(OR(F11&lt;0,F11&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F11&lt;&gt;ROUND(F11,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O11" s="15" t="str">
-        <f>IF(G11="","",IF(G11&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G11&lt;&gt;ROUND(G11,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P11" s="15" t="str">
-        <f>IF(H11="","",IF(H11&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H11&lt;&gt;ROUND(H11,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S11" s="16" t="str">
-        <f>IF(L11="",IF(D11&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2816,41 +2816,41 @@
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="58"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="33"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="49" t="str">
+      <c r="I12" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J12" s="47"/>
+      <c r="K12" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="15" t="str">
-        <f>IF(C12="","",IF(OR(C12&lt;0,C12&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C12&lt;&gt;ROUND(C12,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L12" s="15" t="str">
-        <f>IF(D12="","",IF(D12&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D12&lt;&gt;ROUND(D12,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M12" s="15" t="str">
-        <f>IF(E12="","",IF(E12&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E12&lt;&gt;ROUND(E12,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N12" s="15" t="str">
-        <f>IF(F12="","",IF(OR(F12&lt;0,F12&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F12&lt;&gt;ROUND(F12,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O12" s="15" t="str">
-        <f>IF(G12="","",IF(G12&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G12&lt;&gt;ROUND(G12,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P12" s="15" t="str">
-        <f>IF(H12="","",IF(H12&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H12&lt;&gt;ROUND(H12,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S12" s="16" t="str">
-        <f>IF(L12="",IF(D12&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2863,41 +2863,41 @@
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="58"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="33"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="49" t="str">
+      <c r="I13" s="46" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J13" s="47"/>
+      <c r="K13" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J13" s="50"/>
-      <c r="K13" s="15" t="str">
-        <f>IF(C13="","",IF(OR(C13&lt;0,C13&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C13&lt;&gt;ROUND(C13,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L13" s="15" t="str">
-        <f>IF(D13="","",IF(D13&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D13&lt;&gt;ROUND(D13,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M13" s="15" t="str">
-        <f>IF(E13="","",IF(E13&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E13&lt;&gt;ROUND(E13,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N13" s="15" t="str">
-        <f>IF(F13="","",IF(OR(F13&lt;0,F13&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F13&lt;&gt;ROUND(F13,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O13" s="15" t="str">
-        <f>IF(G13="","",IF(G13&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G13&lt;&gt;ROUND(G13,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P13" s="15" t="str">
-        <f>IF(H13="","",IF(H13&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H13&lt;&gt;ROUND(H13,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S13" s="16" t="str">
-        <f>IF(L13="",IF(D13&gt;65,"加權平均貸款成數最高為6.5成,",""),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -2916,7 +2916,7 @@
         <f>IF(C14=0,0,ROUND(SUMPRODUCT(C7:C13,D7:D13)/C14,2))</f>
         <v>0</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="42">
         <f>$E$13</f>
         <v>0</v>
       </c>
@@ -2933,32 +2933,32 @@
         <v>0</v>
       </c>
       <c r="I14" s="48" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J14" s="49"/>
+      <c r="K14" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J14" s="51"/>
-      <c r="K14" s="15" t="str">
-        <f>IF(C14="","",IF(OR(C14&lt;0,C14&gt;99999999.99),"109.12.8~110.9.23申請案件[撥款金額]須為小於9位之正數,",IF(C14&lt;&gt;ROUND(C14,2),"109.12.8~110.9.23申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
-        <v/>
-      </c>
       <c r="L14" s="15" t="str">
-        <f>IF(D14="","",IF(D14&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(D14&lt;&gt;ROUND(D14,2),"109.12.8~110.9.23申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M14" s="15" t="str">
-        <f>IF(E14="","",IF(E14&gt;99.99,"109.12.8~110.9.23申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(E14&lt;&gt;ROUND(E14,2),"109.12.8~110.9.23申請案件[加權平均貸款利率]小數位數至多為2位,","")))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N14" s="15" t="str">
-        <f>IF(F14="","",IF(OR(F14&lt;0,F14&gt;99999999.99),"110.9.24起申請案件[撥款金額]須為小於9位之正數,",IF(F14&lt;&gt;ROUND(F14,2),"110.9.24起申請案件[撥款金額]須四捨五入至小數下2位,","")))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O14" s="15" t="str">
-        <f>IF(G14="","",IF(G14&gt;99.99,"110.9.24起申請案件[加權平均貸款成數]整數位數須小於3位數,",IF(G14&lt;&gt;ROUND(G14,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P14" s="15" t="str">
-        <f>IF(H14="","",IF(H14&gt;99.99,"110.9.24起申請案件[加權平均貸款利率]整數位數須小於3位數,",IF(H14&lt;&gt;ROUND(H14,2),"110.9.24起申請案件[加權平均貸款成數]小數位數至多為2位,","")))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R14" s="25" t="str">
@@ -2975,13 +2975,13 @@
       </c>
     </row>
     <row r="15" spans="1:68" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
       <c r="S15" s="29"/>
     </row>
     <row r="16" spans="1:68" ht="19.8" x14ac:dyDescent="0.4">
@@ -2997,7 +2997,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="40"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
@@ -3012,7 +3012,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="40"/>
+      <c r="G17" s="35"/>
     </row>
     <row r="18" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
@@ -3027,7 +3027,7 @@
         <v>15</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="40"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
@@ -3061,6 +3061,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="I12:J12"/>
@@ -3073,14 +3081,6 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3120,12 +3120,12 @@
         <f>IF(COUNTBLANK(F5:F12)=8,"","本表有誤")</f>
         <v/>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
       <c r="BA1" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(C2," ",""),"　","")</f>
         <v>民國年月</v>
@@ -3163,10 +3163,10 @@
       </c>
     </row>
     <row r="2" spans="1:62" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:62" s="13" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3473,13 +3473,13 @@
       </c>
     </row>
     <row r="13" spans="1:62" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
       <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:62" ht="19.8" x14ac:dyDescent="0.4">

</xml_diff>